<commit_message>
Penambahan if else dan memperbaiki source code status
</commit_message>
<xml_diff>
--- a/DataDrivenAlfa.xlsx
+++ b/DataDrivenAlfa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Katalon Studio\AlfaCart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D6052C-2A70-4920-A560-84FCF4A6241C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF95F48-38B2-41FD-978F-52C24EE28598}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B8B6F939-D73B-4586-8C53-487560800F88}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Nama</t>
   </si>
@@ -63,13 +63,16 @@
     <t>Login Sukses</t>
   </si>
   <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>Akun Anda untuk sementara tidak dapat digunakan untuk berbelanj</t>
+  </si>
+  <si>
     <t>Invalid email/phone number or password</t>
-  </si>
-  <si>
-    <t>actual</t>
-  </si>
-  <si>
-    <t>expected</t>
   </si>
   <si>
     <t>Akun Anda untuk sementara tidak dapat digunakan untuk berbelanja.</t>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8769099-1B37-4F20-816A-9B8272D3F7C9}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,10 +465,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -479,7 +482,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -493,7 +496,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -508,12 +511,27 @@
       </c>
       <c r="D4" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{18749EFF-817E-4F82-8A11-3EDC92CB05EB}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{6ABB2668-44F4-46E7-82C7-0D05C8771ED9}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{C556D689-C59A-4434-81F4-66BCB3DB0C9E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Penambahan Testing Apps Mobile Android
</commit_message>
<xml_diff>
--- a/DataDrivenAlfa.xlsx
+++ b/DataDrivenAlfa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Katalon Studio\AlfaCart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF95F48-38B2-41FD-978F-52C24EE28598}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE69A620-3BF4-4652-8464-0E6667FAE2AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B8B6F939-D73B-4586-8C53-487560800F88}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Nama</t>
   </si>
@@ -60,22 +60,28 @@
     <t>Cynthia</t>
   </si>
   <si>
-    <t>Login Sukses</t>
-  </si>
-  <si>
     <t>actual</t>
   </si>
   <si>
     <t>expected</t>
   </si>
   <si>
-    <t>Akun Anda untuk sementara tidak dapat digunakan untuk berbelanj</t>
-  </si>
-  <si>
     <t>Invalid email/phone number or password</t>
   </si>
   <si>
     <t>Akun Anda untuk sementara tidak dapat digunakan untuk berbelanja.</t>
+  </si>
+  <si>
+    <t>0816555895</t>
+  </si>
+  <si>
+    <t>Login Success Go To page Profile</t>
+  </si>
+  <si>
+    <t>TestingQA123</t>
+  </si>
+  <si>
+    <t>86772272121</t>
   </si>
 </sst>
 </file>
@@ -107,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -115,14 +121,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -441,13 +464,14 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -465,73 +489,73 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>86772272121</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{18749EFF-817E-4F82-8A11-3EDC92CB05EB}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{6ABB2668-44F4-46E7-82C7-0D05C8771ED9}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{C556D689-C59A-4434-81F4-66BCB3DB0C9E}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{B8ABEA10-10A0-4587-A3A4-036CC4CA1C00}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{DD4ACC33-CE9A-4549-8E17-5AD3BF7F13E8}"/>
+    <hyperlink ref="B2" r:id="rId3" display="hilmi.falih@yahoo.com" xr:uid="{9E1D4A6B-3BB7-400A-AA1E-FDA6235B408C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>